<commit_message>
Day 6 pair + sublime_setup
</commit_message>
<xml_diff>
--- a/DFS/DSA Cracker Sheet 450.xlsx
+++ b/DFS/DSA Cracker Sheet 450.xlsx
@@ -1666,10 +1666,10 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="123"/>
@@ -1732,7 +1732,7 @@
         <v>10</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>